<commit_message>
all ACC-PAG and ACC-ACC neurons + capacitance added
</commit_message>
<xml_diff>
--- a/Data/in/Retro_ACC_PAG.xlsx
+++ b/Data/in/Retro_ACC_PAG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\documents\Repositories\gini\Data\in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AE3B93-6C57-40FA-B709-6C774D42463F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88F0E5C-F5EE-4238-9E10-6148ED262823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{195E0AFB-190A-439D-8920-FC903F239F74}"/>
+    <workbookView xWindow="1128" yWindow="1956" windowWidth="21336" windowHeight="13488" xr2:uid="{195E0AFB-190A-439D-8920-FC903F239F74}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="70">
   <si>
     <t>Label</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>t3</t>
+  </si>
+  <si>
+    <t>Capacitance</t>
   </si>
 </sst>
 </file>
@@ -316,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -341,6 +344,7 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F27D14E-5218-4C12-A051-D8A9399440F5}">
-  <dimension ref="A1:AR52"/>
+  <dimension ref="A1:AR55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R54" sqref="R54"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="56" zoomScaleNormal="56" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42:AN55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -746,34 +750,37 @@
       <c r="Z1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AA1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AC1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AD1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AE1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AF1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AG1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="7" t="s">
+      <c r="AH1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AI1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" s="6" t="s">
+      <c r="AJ1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AK1" s="5" t="s">
         <v>61</v>
       </c>
     </row>
@@ -803,15 +810,15 @@
       <c r="X2" s="6"/>
       <c r="Y2" s="6"/>
       <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
       <c r="AB2" s="6"/>
       <c r="AC2" s="6"/>
       <c r="AD2" s="6"/>
       <c r="AE2" s="6"/>
       <c r="AF2" s="6"/>
-      <c r="AG2" s="7"/>
-      <c r="AH2" s="6"/>
+      <c r="AG2" s="6"/>
+      <c r="AH2" s="7"/>
       <c r="AI2" s="6"/>
+      <c r="AJ2" s="6"/>
     </row>
     <row r="3" spans="1:44" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -892,28 +899,30 @@
       <c r="Z3" s="1">
         <v>9.3873375630055289</v>
       </c>
-      <c r="AA3" s="1">
+      <c r="AA3" s="18">
+        <v>8.4610859289579232E-2</v>
+      </c>
+      <c r="AB3" s="1">
         <v>0.64740566037735858</v>
       </c>
-      <c r="AC3" s="1">
+      <c r="AD3" s="1">
         <v>96.632637023925781</v>
       </c>
-      <c r="AD3" s="1">
+      <c r="AE3" s="1">
         <v>0.88588325635726584</v>
       </c>
-      <c r="AE3" s="1">
+      <c r="AF3" s="1">
         <v>219.27360153198242</v>
       </c>
-      <c r="AF3" s="1">
+      <c r="AG3" s="1">
         <v>94.473598480224609</v>
       </c>
-      <c r="AH3" s="1">
+      <c r="AI3" s="1">
         <v>141.59292035398229</v>
       </c>
-      <c r="AJ3" s="14">
+      <c r="AK3" s="14">
         <v>7.3</v>
       </c>
-      <c r="AK3" s="8"/>
       <c r="AL3" s="8"/>
       <c r="AM3" s="8"/>
       <c r="AN3" s="8"/>
@@ -1002,30 +1011,32 @@
         <v>12.768731151494228</v>
       </c>
       <c r="AA4" s="1">
+        <v>0.11117009879341999</v>
+      </c>
+      <c r="AB4" s="1">
         <v>0.40902474526928667</v>
       </c>
-      <c r="AC4" s="1">
+      <c r="AD4" s="1">
         <v>94.33631706237793</v>
       </c>
-      <c r="AD4" s="1">
+      <c r="AE4" s="1">
         <v>0.89042720860052071</v>
       </c>
-      <c r="AE4" s="1">
+      <c r="AF4" s="1">
         <v>215.27999114990234</v>
       </c>
-      <c r="AF4" s="1">
+      <c r="AG4" s="1">
         <v>86.611198902130127</v>
       </c>
-      <c r="AG4" s="1">
+      <c r="AH4" s="1">
         <v>0.31200027465820313</v>
       </c>
-      <c r="AH4" s="1">
+      <c r="AI4" s="1">
         <v>149.53271028037383</v>
       </c>
-      <c r="AJ4" s="11">
+      <c r="AK4" s="11">
         <v>7.6752000000000002</v>
       </c>
-      <c r="AK4" s="9"/>
       <c r="AL4" s="9"/>
       <c r="AM4" s="9"/>
       <c r="AN4" s="9"/>
@@ -1114,30 +1125,32 @@
         <v>10.434346714627889</v>
       </c>
       <c r="AA5" s="1">
+        <v>6.5456862131306359E-2</v>
+      </c>
+      <c r="AB5" s="1">
         <v>0.44479004665629862</v>
       </c>
-      <c r="AC5" s="1">
+      <c r="AD5" s="1">
         <v>102.34319569514349</v>
       </c>
-      <c r="AD5" s="1">
+      <c r="AE5" s="1">
         <v>0.98764887984519156</v>
       </c>
-      <c r="AE5" s="1">
+      <c r="AF5" s="1">
         <v>20659.235712443769</v>
       </c>
-      <c r="AF5" s="1">
+      <c r="AG5" s="1">
         <v>246.35519409179688</v>
       </c>
-      <c r="AG5" s="1">
+      <c r="AH5" s="1">
         <v>80.745601654052734</v>
       </c>
-      <c r="AH5" s="1">
+      <c r="AI5" s="1">
         <v>129.03225806451613</v>
       </c>
-      <c r="AJ5" s="15">
+      <c r="AK5" s="15">
         <v>8.5488</v>
       </c>
-      <c r="AK5" s="9"/>
       <c r="AL5" s="9"/>
       <c r="AM5" s="9"/>
       <c r="AN5" s="9"/>
@@ -1226,27 +1239,29 @@
         <v>9.2378725548882255</v>
       </c>
       <c r="AA6" s="1">
+        <v>9.709848154465249E-2</v>
+      </c>
+      <c r="AB6" s="1">
         <v>0.1075268817204301</v>
       </c>
-      <c r="AC6" s="1">
+      <c r="AD6" s="1">
         <v>80.72063751220702</v>
       </c>
-      <c r="AD6" s="1">
+      <c r="AE6" s="1">
         <v>1.1324077066418248</v>
       </c>
-      <c r="AE6" s="1">
+      <c r="AF6" s="1">
         <v>152.2559986114502</v>
       </c>
-      <c r="AF6" s="1">
+      <c r="AG6" s="1">
         <v>63.148798942565918</v>
       </c>
-      <c r="AH6" s="1">
+      <c r="AI6" s="1">
         <v>166.66666666666669</v>
       </c>
-      <c r="AJ6" s="11">
+      <c r="AK6" s="11">
         <v>6.8639999999999999</v>
       </c>
-      <c r="AK6" s="9"/>
       <c r="AL6" s="9"/>
       <c r="AM6" s="9"/>
       <c r="AN6" s="9"/>
@@ -1334,28 +1349,30 @@
       <c r="Z7" s="2">
         <v>3.8772849582433357</v>
       </c>
-      <c r="AA7" s="2">
+      <c r="AA7" s="1">
+        <v>4.9132296358992245E-2</v>
+      </c>
+      <c r="AB7" s="2">
         <v>0.13219094247246022</v>
       </c>
-      <c r="AC7" s="2">
+      <c r="AD7" s="2">
         <v>80.689438629150388</v>
       </c>
-      <c r="AD7" s="2">
+      <c r="AE7" s="2">
         <v>1.1682877450307139</v>
       </c>
-      <c r="AE7" s="2">
+      <c r="AF7" s="2">
         <v>143.39520072937012</v>
       </c>
-      <c r="AF7" s="2">
+      <c r="AG7" s="2">
         <v>58.406397819519043</v>
       </c>
-      <c r="AH7" s="2">
+      <c r="AI7" s="2">
         <v>176.99115044247787</v>
       </c>
-      <c r="AJ7" s="11">
+      <c r="AK7" s="11">
         <v>8.4239999999999995</v>
       </c>
-      <c r="AK7" s="9"/>
       <c r="AL7" s="9"/>
       <c r="AM7" s="9"/>
       <c r="AN7" s="9"/>
@@ -1444,30 +1461,32 @@
         <v>4.2619707854089475</v>
       </c>
       <c r="AA8" s="2">
+        <v>4.4679989699251521E-2</v>
+      </c>
+      <c r="AB8" s="2">
         <v>0.28003696857670984</v>
       </c>
-      <c r="AC8" s="2">
+      <c r="AD8" s="2">
         <v>74.655358123779294</v>
       </c>
-      <c r="AD8" s="2">
+      <c r="AE8" s="2">
         <v>1.2928535915563515</v>
       </c>
-      <c r="AE8" s="2">
+      <c r="AF8" s="2">
         <v>129.91680145263672</v>
       </c>
-      <c r="AF8" s="2">
+      <c r="AG8" s="2">
         <v>55.161599308252335</v>
       </c>
-      <c r="AG8" s="2">
+      <c r="AH8" s="2">
         <v>2.5271987915039063</v>
       </c>
-      <c r="AH8" s="2">
+      <c r="AI8" s="2">
         <v>115.46391752577317</v>
       </c>
-      <c r="AJ8" s="12">
+      <c r="AK8" s="12">
         <v>8.2368000000000006</v>
       </c>
-      <c r="AK8" s="10"/>
       <c r="AL8" s="10"/>
       <c r="AM8" s="10"/>
       <c r="AN8" s="10"/>
@@ -1555,31 +1574,33 @@
       <c r="Z9" s="3">
         <v>9.3973171439373804</v>
       </c>
-      <c r="AA9" s="3">
+      <c r="AA9" s="2">
+        <v>9.3403780741572628E-2</v>
+      </c>
+      <c r="AB9" s="3">
         <v>0.42873432155074115</v>
       </c>
-      <c r="AC9" s="3">
+      <c r="AD9" s="3">
         <v>85.475517272949219</v>
       </c>
-      <c r="AD9" s="3">
+      <c r="AE9" s="3">
         <v>1.3841862989679043</v>
       </c>
-      <c r="AE9" s="3">
+      <c r="AF9" s="3">
         <v>134.28479385375977</v>
       </c>
-      <c r="AF9" s="3">
+      <c r="AG9" s="3">
         <v>53.164798736572266</v>
       </c>
-      <c r="AG9" s="3">
+      <c r="AH9" s="3">
         <v>13.946399688720703</v>
       </c>
-      <c r="AH9" s="2">
+      <c r="AI9" s="2">
         <v>238.80597014925371</v>
       </c>
-      <c r="AJ9" s="12">
+      <c r="AK9" s="12">
         <v>6.8015999999999996</v>
       </c>
-      <c r="AK9" s="10"/>
       <c r="AL9" s="10"/>
       <c r="AM9" s="10"/>
       <c r="AN9" s="10"/>
@@ -1667,31 +1688,33 @@
       <c r="Z10" s="3">
         <v>9.2598681789534449</v>
       </c>
-      <c r="AA10" s="3">
+      <c r="AA10" s="2">
+        <v>9.2882524146701104E-2</v>
+      </c>
+      <c r="AB10" s="3">
         <v>0.65454545454545454</v>
       </c>
-      <c r="AC10" s="3">
+      <c r="AD10" s="3">
         <v>76.764478874206546</v>
       </c>
-      <c r="AD10" s="3">
+      <c r="AE10" s="3">
         <v>1.1271616263761963</v>
       </c>
-      <c r="AE10" s="3">
+      <c r="AF10" s="3">
         <v>117.93599605560303</v>
       </c>
-      <c r="AF10" s="3">
+      <c r="AG10" s="3">
         <v>50.793597221374512</v>
       </c>
-      <c r="AG10" s="3">
+      <c r="AH10" s="3">
         <v>2.683197021484375</v>
       </c>
-      <c r="AH10" s="2">
+      <c r="AI10" s="2">
         <v>0</v>
       </c>
-      <c r="AJ10" s="12">
+      <c r="AK10" s="12">
         <v>4.3368000000000002</v>
       </c>
-      <c r="AK10" s="10"/>
       <c r="AL10" s="10"/>
       <c r="AM10" s="10"/>
       <c r="AN10" s="10"/>
@@ -1779,31 +1802,33 @@
       <c r="Z11" s="3">
         <v>6.2599989481466674</v>
       </c>
-      <c r="AA11" s="3">
+      <c r="AA11" s="2">
+        <v>5.8518661944116805E-2</v>
+      </c>
+      <c r="AB11" s="3">
         <v>0.57412935323383085</v>
       </c>
-      <c r="AC11" s="3">
+      <c r="AD11" s="3">
         <v>76.078076267242437</v>
       </c>
-      <c r="AD11" s="3">
+      <c r="AE11" s="3">
         <v>1.0594391524923523</v>
       </c>
-      <c r="AE11" s="3">
+      <c r="AF11" s="3">
         <v>143.02078819274902</v>
       </c>
-      <c r="AF11" s="3">
+      <c r="AG11" s="3">
         <v>59.779199600219727</v>
       </c>
-      <c r="AG11" s="3">
+      <c r="AH11" s="3">
         <v>1.3416023254394531</v>
       </c>
-      <c r="AH11" s="3">
+      <c r="AI11" s="3">
         <v>271.18644067796612</v>
       </c>
-      <c r="AJ11" s="12">
+      <c r="AK11" s="12">
         <v>5.7408000000000001</v>
       </c>
-      <c r="AK11" s="10"/>
       <c r="AL11" s="10"/>
       <c r="AM11" s="10"/>
       <c r="AN11" s="10"/>
@@ -1891,31 +1916,33 @@
       <c r="Z12" s="1">
         <v>10.86035989853354</v>
       </c>
-      <c r="AA12" s="1">
+      <c r="AA12" s="2">
+        <v>8.2957211678098164E-2</v>
+      </c>
+      <c r="AB12" s="1">
         <v>0.31731984829329962</v>
       </c>
-      <c r="AC12" s="1">
+      <c r="AD12" s="1">
         <v>112.04543991088866</v>
       </c>
-      <c r="AD12" s="1">
+      <c r="AE12" s="1">
         <v>1.1163522867198807</v>
       </c>
-      <c r="AE12" s="1">
+      <c r="AF12" s="1">
         <v>203.79839324951172</v>
       </c>
-      <c r="AF12" s="1">
+      <c r="AG12" s="1">
         <v>69.763202667236328</v>
       </c>
-      <c r="AG12" s="1">
+      <c r="AH12" s="1">
         <v>2.1215972900390625</v>
       </c>
-      <c r="AH12" s="1">
+      <c r="AI12" s="1">
         <v>197.53086419753089</v>
       </c>
-      <c r="AJ12" s="12">
+      <c r="AK12" s="12">
         <v>9.5784000000000002</v>
       </c>
-      <c r="AK12" s="10"/>
       <c r="AL12" s="10"/>
       <c r="AM12" s="10"/>
       <c r="AN12" s="10"/>
@@ -2004,30 +2031,32 @@
         <v>9.8054583081365259</v>
       </c>
       <c r="AA13" s="1">
+        <v>8.2668360789136155E-2</v>
+      </c>
+      <c r="AB13" s="1">
         <v>0.44677419354838716</v>
       </c>
-      <c r="AC13" s="1">
+      <c r="AD13" s="1">
         <v>94.769998550415039</v>
       </c>
-      <c r="AD13" s="1">
+      <c r="AE13" s="1">
         <v>1.0927261019959289</v>
       </c>
-      <c r="AE13" s="1">
+      <c r="AF13" s="1">
         <v>174.09599685668945</v>
       </c>
-      <c r="AF13" s="1">
+      <c r="AG13" s="1">
         <v>79.497596740722656</v>
       </c>
-      <c r="AG13" s="1">
+      <c r="AH13" s="1">
         <v>2.93280029296875</v>
       </c>
-      <c r="AH13" s="1">
+      <c r="AI13" s="1">
         <v>242.42424242424241</v>
       </c>
-      <c r="AJ13" s="11">
+      <c r="AK13" s="11">
         <v>5.3040000000000003</v>
       </c>
-      <c r="AK13" s="9"/>
       <c r="AL13" s="9"/>
       <c r="AM13" s="9"/>
       <c r="AN13" s="9"/>
@@ -2116,30 +2145,32 @@
         <v>7.8400207207263861</v>
       </c>
       <c r="AA14" s="1">
+        <v>0.13553547426361454</v>
+      </c>
+      <c r="AB14" s="1">
         <v>0.6560509554140127</v>
       </c>
-      <c r="AC14" s="1">
+      <c r="AD14" s="1">
         <v>99.989756774902332</v>
       </c>
-      <c r="AD14" s="1">
+      <c r="AE14" s="1">
         <v>1.1107206014497741</v>
       </c>
-      <c r="AE14" s="1">
+      <c r="AF14" s="1">
         <v>211.53599548339844</v>
       </c>
-      <c r="AF14" s="1">
+      <c r="AG14" s="1">
         <v>80.121597290039063</v>
       </c>
-      <c r="AG14" s="1">
+      <c r="AH14" s="1">
         <v>1.3103981018066406</v>
       </c>
-      <c r="AH14" s="1">
+      <c r="AI14" s="1">
         <v>0</v>
       </c>
-      <c r="AJ14" s="11">
+      <c r="AK14" s="11">
         <v>3.2136</v>
       </c>
-      <c r="AK14" s="9"/>
       <c r="AL14" s="9"/>
       <c r="AM14" s="9"/>
       <c r="AN14" s="9"/>
@@ -2228,27 +2259,29 @@
         <v>7.4624086723082632</v>
       </c>
       <c r="AA15" s="1">
+        <v>5.246321257879745E-2</v>
+      </c>
+      <c r="AB15" s="1">
         <v>0.57171117705242325</v>
       </c>
-      <c r="AC15" s="1">
+      <c r="AD15" s="1">
         <v>96.417357635498036</v>
       </c>
-      <c r="AD15" s="1">
+      <c r="AE15" s="1">
         <v>0.94149861686122449</v>
       </c>
-      <c r="AE15" s="1">
+      <c r="AF15" s="1">
         <v>207.41759490966797</v>
       </c>
-      <c r="AF15" s="1">
+      <c r="AG15" s="1">
         <v>89.481594085693359</v>
       </c>
-      <c r="AH15" s="1">
+      <c r="AI15" s="1">
         <v>238.80597014925371</v>
       </c>
-      <c r="AJ15" s="11">
+      <c r="AK15" s="11">
         <v>11.638</v>
       </c>
-      <c r="AK15" s="9"/>
       <c r="AL15" s="9"/>
       <c r="AM15" s="9"/>
       <c r="AN15" s="9"/>
@@ -2337,30 +2370,32 @@
         <v>8.629055300021065</v>
       </c>
       <c r="AA16" s="1">
+        <v>0.10761568456302112</v>
+      </c>
+      <c r="AB16" s="1">
         <v>0.35352422907488984</v>
       </c>
-      <c r="AC16" s="1">
+      <c r="AD16" s="1">
         <v>102.14879684448243</v>
       </c>
-      <c r="AD16" s="1">
+      <c r="AE16" s="1">
         <v>1.2178108241504688</v>
       </c>
-      <c r="AE16" s="1">
+      <c r="AF16" s="1">
         <v>198.43199157714844</v>
       </c>
-      <c r="AF16" s="1">
+      <c r="AG16" s="1">
         <v>63.523200035095215</v>
       </c>
-      <c r="AG16" s="1">
+      <c r="AH16" s="1">
         <v>6.302398681640625</v>
       </c>
-      <c r="AH16" s="1">
+      <c r="AI16" s="1">
         <v>164.94845360824741</v>
       </c>
-      <c r="AJ16" s="11">
+      <c r="AK16" s="11">
         <v>10.358000000000001</v>
       </c>
-      <c r="AK16" s="9"/>
       <c r="AL16" s="9"/>
       <c r="AM16" s="9"/>
       <c r="AN16" s="9"/>
@@ -2449,30 +2484,32 @@
         <v>8.3432087808633</v>
       </c>
       <c r="AA17" s="1">
+        <v>9.1131618695540123E-2</v>
+      </c>
+      <c r="AB17" s="1">
         <v>0.63364485981308405</v>
       </c>
-      <c r="AC17" s="1">
+      <c r="AD17" s="1">
         <v>88.224238967895502</v>
       </c>
-      <c r="AD17" s="1">
+      <c r="AE17" s="1">
         <v>1.4282470020051896</v>
       </c>
-      <c r="AE17" s="1">
+      <c r="AF17" s="1">
         <v>158.62080001831055</v>
       </c>
-      <c r="AF17" s="1">
+      <c r="AG17" s="1">
         <v>45.801598072052002</v>
       </c>
-      <c r="AG17" s="1">
+      <c r="AH17" s="1">
         <v>0.28079986572265625</v>
       </c>
-      <c r="AH17" s="1">
+      <c r="AI17" s="1">
         <v>0</v>
       </c>
-      <c r="AJ17" s="11">
+      <c r="AK17" s="11">
         <v>5.0544000000000002</v>
       </c>
-      <c r="AK17" s="9"/>
       <c r="AL17" s="9"/>
       <c r="AM17" s="9"/>
       <c r="AN17" s="9"/>
@@ -2561,27 +2598,29 @@
         <v>32.497838930464667</v>
       </c>
       <c r="AA18" s="1">
+        <v>0.22993321189775917</v>
+      </c>
+      <c r="AB18" s="1">
         <v>0.40428571428571425</v>
       </c>
-      <c r="AC18" s="1">
+      <c r="AD18" s="1">
         <v>106.14239578247071</v>
       </c>
-      <c r="AD18" s="1">
+      <c r="AE18" s="1">
         <v>1.1797852560458759</v>
       </c>
-      <c r="AE18" s="1">
+      <c r="AF18" s="1">
         <v>272.43840026855469</v>
       </c>
-      <c r="AF18" s="1">
+      <c r="AG18" s="1">
         <v>75.753599166870117</v>
       </c>
-      <c r="AH18" s="1">
+      <c r="AI18" s="1">
         <v>147.23926380368098</v>
       </c>
-      <c r="AJ18" s="15">
+      <c r="AK18" s="15">
         <v>4.1807999999999996</v>
       </c>
-      <c r="AK18" s="9"/>
       <c r="AL18" s="9"/>
       <c r="AM18" s="9"/>
       <c r="AN18" s="9"/>
@@ -2670,27 +2709,29 @@
         <v>7.3633163133105857</v>
       </c>
       <c r="AA19" s="1">
+        <v>0.12117255481046554</v>
+      </c>
+      <c r="AB19" s="1">
         <v>0.12285714285714286</v>
       </c>
-      <c r="AC19" s="1">
+      <c r="AD19" s="1">
         <v>114.99383659362792</v>
       </c>
-      <c r="AD19" s="1">
+      <c r="AE19" s="1">
         <v>0.95247443763236816</v>
       </c>
-      <c r="AE19" s="1">
+      <c r="AF19" s="1">
         <v>292.78079223632813</v>
       </c>
-      <c r="AF19" s="1">
+      <c r="AG19" s="1">
         <v>88.233596801757813</v>
       </c>
-      <c r="AH19" s="1">
+      <c r="AI19" s="1">
         <v>140.35087719298244</v>
       </c>
-      <c r="AJ19" s="11">
+      <c r="AK19" s="11">
         <v>6.6768000000000001</v>
       </c>
-      <c r="AK19" s="9"/>
       <c r="AL19" s="9"/>
       <c r="AM19" s="9"/>
       <c r="AN19" s="9"/>
@@ -2779,30 +2820,32 @@
         <v>11.158352792537027</v>
       </c>
       <c r="AA20" s="1">
+        <v>0.10798294044869483</v>
+      </c>
+      <c r="AB20" s="1">
         <v>0.59379844961240313</v>
       </c>
-      <c r="AC20" s="1">
+      <c r="AD20" s="1">
         <v>114.17327804565429</v>
       </c>
-      <c r="AD20" s="1">
+      <c r="AE20" s="1">
         <v>0.97610023244142496</v>
       </c>
-      <c r="AE20" s="1">
+      <c r="AF20" s="1">
         <v>241.23838806152344</v>
       </c>
-      <c r="AF20" s="1">
+      <c r="AG20" s="1">
         <v>86.486398696899414</v>
       </c>
-      <c r="AG20" s="1">
+      <c r="AH20" s="1">
         <v>1.4351997375488281</v>
       </c>
-      <c r="AH20" s="1">
+      <c r="AI20" s="1">
         <v>0</v>
       </c>
-      <c r="AJ20" s="11">
+      <c r="AK20" s="11">
         <v>7.1135999999999999</v>
       </c>
-      <c r="AK20" s="9"/>
       <c r="AL20" s="9"/>
       <c r="AM20" s="9"/>
       <c r="AN20" s="9"/>
@@ -2891,27 +2934,29 @@
         <v>10.695772072547435</v>
       </c>
       <c r="AA21" s="1">
+        <v>6.125312226122321E-2</v>
+      </c>
+      <c r="AB21" s="1">
         <v>0</v>
       </c>
-      <c r="AC21" s="1">
+      <c r="AD21" s="1">
         <v>80.87351722717284</v>
       </c>
-      <c r="AD21" s="1">
+      <c r="AE21" s="1">
         <v>1.0659451613782949</v>
       </c>
-      <c r="AE21" s="1">
+      <c r="AF21" s="1">
         <v>157.12319660186768</v>
       </c>
-      <c r="AF21" s="1">
+      <c r="AG21" s="1">
         <v>75.503997802734375</v>
       </c>
-      <c r="AH21" s="1">
+      <c r="AI21" s="1">
         <v>0</v>
       </c>
-      <c r="AJ21" s="11">
+      <c r="AK21" s="11">
         <v>1.1856</v>
       </c>
-      <c r="AK21" s="9"/>
       <c r="AL21" s="9"/>
       <c r="AM21" s="9"/>
       <c r="AN21" s="9"/>
@@ -3000,27 +3045,29 @@
         <v>7.9005049636582303</v>
       </c>
       <c r="AA22" s="1">
+        <v>4.1924066222939621E-2</v>
+      </c>
+      <c r="AB22" s="1">
         <v>0</v>
       </c>
-      <c r="AC22" s="1">
+      <c r="AD22" s="1">
         <v>98.336158370971674</v>
       </c>
-      <c r="AD22" s="1">
+      <c r="AE22" s="1">
         <v>1.7836296256680839</v>
       </c>
-      <c r="AE22" s="1">
+      <c r="AF22" s="1">
         <v>147.38879585266113</v>
       </c>
-      <c r="AF22" s="1">
+      <c r="AG22" s="1">
         <v>41.184000253677368</v>
       </c>
-      <c r="AH22" s="1">
+      <c r="AI22" s="1">
         <v>0</v>
       </c>
-      <c r="AJ22" s="11">
+      <c r="AK22" s="11">
         <v>2.5583999999999998</v>
       </c>
-      <c r="AK22" s="9"/>
       <c r="AL22" s="9"/>
       <c r="AM22" s="9"/>
       <c r="AN22" s="9"/>
@@ -3109,30 +3156,32 @@
         <v>15.063201172258813</v>
       </c>
       <c r="AA23" s="1">
+        <v>0.3506136509397651</v>
+      </c>
+      <c r="AB23" s="1">
         <v>0.76903870162297139</v>
       </c>
-      <c r="AC23" s="1">
+      <c r="AD23" s="1">
         <v>87.481678009033203</v>
       </c>
-      <c r="AD23" s="1">
+      <c r="AE23" s="1">
         <v>0.88464292543460488</v>
       </c>
-      <c r="AE23" s="1">
+      <c r="AF23" s="1">
         <v>194.56319427490234</v>
       </c>
-      <c r="AF23" s="1">
+      <c r="AG23" s="1">
         <v>91.977596282958984</v>
       </c>
-      <c r="AG23" s="1">
+      <c r="AH23" s="1">
         <v>1.1543998718261719</v>
       </c>
-      <c r="AH23" s="1">
+      <c r="AI23" s="1">
         <v>0</v>
       </c>
-      <c r="AJ23" s="11">
+      <c r="AK23" s="11">
         <v>2.4024000000000001</v>
       </c>
-      <c r="AK23" s="9"/>
       <c r="AL23" s="9"/>
       <c r="AM23" s="9"/>
       <c r="AN23" s="9"/>
@@ -3221,30 +3270,32 @@
         <v>9.4185301100910408</v>
       </c>
       <c r="AA24" s="4">
+        <v>6.1893650289496845E-2</v>
+      </c>
+      <c r="AB24" s="4">
         <v>0.7065693430656933</v>
       </c>
-      <c r="AC24" s="4">
+      <c r="AD24" s="4">
         <v>86.636157989501953</v>
       </c>
-      <c r="AD24" s="4">
+      <c r="AE24" s="4">
         <v>1.97248012626554</v>
       </c>
-      <c r="AE24" s="4">
+      <c r="AF24" s="4">
         <v>142.64639610052109</v>
       </c>
-      <c r="AF24" s="4">
+      <c r="AG24" s="4">
         <v>42.182399749755859</v>
       </c>
-      <c r="AG24" s="4">
+      <c r="AH24" s="4">
         <v>0.1248016357421875</v>
       </c>
-      <c r="AH24" s="4">
+      <c r="AI24" s="4">
         <v>0</v>
       </c>
-      <c r="AJ24" s="13">
+      <c r="AK24" s="13">
         <v>1.0296000000000001</v>
       </c>
-      <c r="AK24" s="9"/>
       <c r="AL24" s="9"/>
       <c r="AM24" s="9"/>
       <c r="AN24" s="9"/>
@@ -3333,27 +3384,29 @@
         <v>9.8872867320181257</v>
       </c>
       <c r="AA25" s="4">
+        <v>8.3984151130049117E-2</v>
+      </c>
+      <c r="AB25" s="4">
         <v>0.81070745697896751</v>
       </c>
-      <c r="AC25" s="4">
+      <c r="AD25" s="4">
         <v>93.506396484374989</v>
       </c>
-      <c r="AD25" s="4">
+      <c r="AE25" s="4">
         <v>1.5643719248002519</v>
       </c>
-      <c r="AE25" s="4">
+      <c r="AF25" s="4">
         <v>174.96959686279297</v>
       </c>
-      <c r="AF25" s="4">
+      <c r="AG25" s="4">
         <v>53.788795471191406</v>
       </c>
-      <c r="AH25" s="4">
+      <c r="AI25" s="4">
         <v>0</v>
       </c>
-      <c r="AJ25" s="13">
+      <c r="AK25" s="13">
         <v>0.78</v>
       </c>
-      <c r="AK25" s="9"/>
       <c r="AL25" s="9"/>
       <c r="AM25" s="9"/>
       <c r="AN25" s="9"/>
@@ -3442,30 +3495,32 @@
         <v>4.9886401172675443</v>
       </c>
       <c r="AA26" s="4">
+        <v>4.9354554685969908E-2</v>
+      </c>
+      <c r="AB26" s="4">
         <v>5.4212454212454221E-2</v>
       </c>
-      <c r="AC26" s="4">
+      <c r="AD26" s="4">
         <v>106.76951904296874</v>
       </c>
-      <c r="AD26" s="4">
+      <c r="AE26" s="4">
         <v>0.83925683923958516</v>
       </c>
-      <c r="AE26" s="4">
+      <c r="AF26" s="4">
         <v>321.23519897460938</v>
       </c>
-      <c r="AF26" s="4">
+      <c r="AG26" s="4">
         <v>102.95999908447266</v>
       </c>
-      <c r="AG26" s="4">
+      <c r="AH26" s="4">
         <v>11.200798034667969</v>
       </c>
-      <c r="AH26" s="4">
+      <c r="AI26" s="4">
         <v>186.04651162790699</v>
       </c>
-      <c r="AJ26" s="13">
+      <c r="AK26" s="13">
         <v>1.0920000000000001</v>
       </c>
-      <c r="AK26" s="9"/>
       <c r="AL26" s="9"/>
       <c r="AM26" s="9"/>
       <c r="AN26" s="9"/>
@@ -3554,27 +3609,29 @@
         <v>10.246226637924767</v>
       </c>
       <c r="AA27" s="4">
+        <v>5.0708431391718982E-2</v>
+      </c>
+      <c r="AB27" s="4">
         <v>0.31034482758620696</v>
       </c>
-      <c r="AC27" s="4">
+      <c r="AD27" s="4">
         <v>118.62551651000976</v>
       </c>
-      <c r="AD27" s="4">
+      <c r="AE27" s="4">
         <v>0.84735450945047042</v>
       </c>
-      <c r="AE27" s="4">
+      <c r="AF27" s="4">
         <v>311.62559509277344</v>
       </c>
-      <c r="AF27" s="4">
+      <c r="AG27" s="4">
         <v>104.45759582519531</v>
       </c>
-      <c r="AH27" s="4">
+      <c r="AI27" s="4">
         <v>121.82741116751269</v>
       </c>
-      <c r="AJ27" s="13">
+      <c r="AK27" s="13">
         <v>2.5895999999999999</v>
       </c>
-      <c r="AK27" s="9"/>
       <c r="AL27" s="9"/>
       <c r="AM27" s="9"/>
       <c r="AN27" s="9"/>
@@ -3663,27 +3720,29 @@
         <v>8.1506892864013452</v>
       </c>
       <c r="AA28" s="4">
+        <v>4.1769448245546813E-2</v>
+      </c>
+      <c r="AB28" s="4">
         <v>0.53238866396761142</v>
       </c>
-      <c r="AC28" s="4">
+      <c r="AD28" s="4">
         <v>95.899437332153326</v>
       </c>
-      <c r="AD28" s="4">
+      <c r="AE28" s="4">
         <v>1.358300225315336</v>
       </c>
-      <c r="AE28" s="4">
+      <c r="AF28" s="4">
         <v>107.20320030000001</v>
       </c>
-      <c r="AF28" s="4">
+      <c r="AG28" s="4">
         <v>46.675198080000001</v>
       </c>
-      <c r="AH28" s="4">
+      <c r="AI28" s="4">
         <v>0</v>
       </c>
-      <c r="AJ28" s="13">
+      <c r="AK28" s="13">
         <v>1.6624000000000001</v>
       </c>
-      <c r="AK28" s="9"/>
       <c r="AL28" s="9"/>
       <c r="AM28" s="9"/>
       <c r="AN28" s="9"/>
@@ -3772,27 +3831,29 @@
         <v>10.558902587300091</v>
       </c>
       <c r="AA29" s="4">
+        <v>5.6442022441044265E-2</v>
+      </c>
+      <c r="AB29" s="4">
         <v>0.65949820788530455</v>
       </c>
-      <c r="AC29" s="4">
+      <c r="AD29" s="4">
         <v>92.264637756347668</v>
       </c>
-      <c r="AD29" s="4">
+      <c r="AE29" s="4">
         <v>1.413222879499644</v>
       </c>
-      <c r="AE29" s="4">
+      <c r="AF29" s="4">
         <v>123.42719649999999</v>
       </c>
-      <c r="AF29" s="4">
+      <c r="AG29" s="4">
         <v>53.913598059999998</v>
       </c>
-      <c r="AH29" s="4">
+      <c r="AI29" s="4">
         <v>0</v>
       </c>
-      <c r="AJ29" s="13">
+      <c r="AK29" s="13">
         <v>1.5911999999999999</v>
       </c>
-      <c r="AK29" s="9"/>
       <c r="AL29" s="9"/>
       <c r="AM29" s="9"/>
       <c r="AN29" s="9"/>
@@ -3881,27 +3942,29 @@
         <v>9.9504443357852672</v>
       </c>
       <c r="AA30" s="4">
+        <v>6.2116054238171216E-2</v>
+      </c>
+      <c r="AB30" s="4">
         <v>0.2521087160262418</v>
       </c>
-      <c r="AC30" s="4">
+      <c r="AD30" s="4">
         <v>115.86743774414063</v>
       </c>
-      <c r="AD30" s="4">
+      <c r="AE30" s="4">
         <v>1.0198239533252433</v>
       </c>
-      <c r="AE30" s="4">
+      <c r="AF30" s="4">
         <v>176.34239959999999</v>
       </c>
-      <c r="AF30" s="4">
+      <c r="AG30" s="4">
         <v>58.780796530000003</v>
       </c>
-      <c r="AH30" s="4">
+      <c r="AI30" s="4">
         <v>216.2162162162162</v>
       </c>
-      <c r="AJ30" s="13">
+      <c r="AK30" s="13">
         <v>0.74880000000000002</v>
       </c>
-      <c r="AK30" s="9"/>
       <c r="AL30" s="9"/>
       <c r="AM30" s="9"/>
       <c r="AN30" s="9"/>
@@ -3920,7 +3983,9 @@
       <c r="C31" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="D31" s="16"/>
+      <c r="D31" s="16">
+        <v>2</v>
+      </c>
       <c r="E31" s="16" t="s">
         <v>34</v>
       </c>
@@ -3982,38 +4047,40 @@
         <v>-66.739918518066403</v>
       </c>
       <c r="Y31" s="17">
-        <v>734.01078086576638</v>
+        <v>73.401078086576604</v>
       </c>
       <c r="Z31" s="17">
         <v>14.598550492505685</v>
       </c>
       <c r="AA31" s="4">
+        <v>0.18003877382284195</v>
+      </c>
+      <c r="AB31" s="4">
         <v>0</v>
       </c>
-      <c r="AB31" s="16"/>
-      <c r="AC31" s="17">
+      <c r="AC31" s="16"/>
+      <c r="AD31" s="17">
         <v>110.63831787109376</v>
       </c>
-      <c r="AD31" s="17">
+      <c r="AE31" s="17">
         <v>1.1524261134964888</v>
       </c>
-      <c r="AE31" s="17">
+      <c r="AF31" s="17">
         <v>204.54719924926758</v>
       </c>
-      <c r="AF31" s="17">
+      <c r="AG31" s="17">
         <v>81.993598937988281</v>
       </c>
-      <c r="AG31" s="17">
+      <c r="AH31" s="17">
         <v>4.3367996215820313</v>
       </c>
-      <c r="AH31" s="4">
+      <c r="AI31" s="4">
         <v>0</v>
       </c>
-      <c r="AI31" s="16"/>
-      <c r="AJ31" s="16">
+      <c r="AJ31" s="16"/>
+      <c r="AK31" s="16">
         <v>0.43081000000000003</v>
       </c>
-      <c r="AK31" s="9"/>
       <c r="AL31" s="9"/>
       <c r="AM31" s="9"/>
       <c r="AN31" s="9"/>
@@ -4032,7 +4099,9 @@
       <c r="C32" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="16"/>
+      <c r="D32" s="16">
+        <v>2</v>
+      </c>
       <c r="E32" s="16" t="s">
         <v>64</v>
       </c>
@@ -4088,45 +4157,48 @@
         <v>3.3384017944335938</v>
       </c>
       <c r="W32" s="17">
-        <v>21.455201466878243</v>
+        <v>214.55201466878199</v>
       </c>
       <c r="X32" s="17">
         <v>-61.579438400268558</v>
       </c>
       <c r="Y32" s="17">
-        <v>178.02064383377206</v>
+        <v>71.8020643833772</v>
       </c>
       <c r="Z32" s="17">
         <v>28.064124724547373</v>
       </c>
       <c r="AA32" s="4">
+        <v>0.13080336145000457</v>
+      </c>
+      <c r="AB32" s="4">
         <v>0</v>
       </c>
-      <c r="AB32" s="16"/>
-      <c r="AC32" s="17">
+      <c r="AC32" s="16"/>
+      <c r="AD32" s="17">
         <v>100.39223594665526</v>
       </c>
-      <c r="AD32" s="17">
+      <c r="AE32" s="17">
         <v>0.96640296866911513</v>
       </c>
-      <c r="AE32" s="17">
+      <c r="AF32" s="17">
         <v>233.87519073486328</v>
       </c>
-      <c r="AF32" s="17">
+      <c r="AG32" s="17">
         <v>89.855995178222656</v>
       </c>
-      <c r="AG32" s="17">
+      <c r="AH32" s="17">
         <v>1.1400032043457</v>
       </c>
-      <c r="AH32" s="4">
+      <c r="AI32" s="4">
         <v>0</v>
       </c>
-      <c r="AI32" s="16"/>
-      <c r="AJ32" s="17">
+      <c r="AJ32" s="16"/>
+      <c r="AK32" s="17">
         <v>1.2791999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>0</v>
       </c>
@@ -4136,7 +4208,9 @@
       <c r="C33" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="D33" s="16"/>
+      <c r="D33" s="16">
+        <v>2</v>
+      </c>
       <c r="E33" s="16" t="s">
         <v>33</v>
       </c>
@@ -4192,45 +4266,48 @@
         <v>0.592803955078125</v>
       </c>
       <c r="W33" s="17">
-        <v>20.872787475585945</v>
+        <v>208.72787475585901</v>
       </c>
       <c r="X33" s="17">
         <v>-66.683758544921872</v>
       </c>
       <c r="Y33" s="17">
-        <v>725.17940791155434</v>
+        <v>72.517940791155397</v>
       </c>
       <c r="Z33" s="17">
         <v>10.95783049103898</v>
       </c>
       <c r="AA33" s="4">
+        <v>5.249816539288743E-2</v>
+      </c>
+      <c r="AB33" s="4">
         <v>0</v>
       </c>
-      <c r="AB33" s="16"/>
-      <c r="AC33" s="17">
+      <c r="AC33" s="16"/>
+      <c r="AD33" s="17">
         <v>103.31255798339845</v>
       </c>
-      <c r="AD33" s="17">
+      <c r="AE33" s="17">
         <v>1.3988190451550651</v>
       </c>
-      <c r="AE33" s="17">
+      <c r="AF33" s="17">
         <v>171.10079193115234</v>
       </c>
-      <c r="AF33" s="17">
+      <c r="AG33" s="17">
         <v>67.142398834228516</v>
       </c>
-      <c r="AG33" s="17">
+      <c r="AH33" s="17">
         <v>4.5551986694335938</v>
       </c>
-      <c r="AH33" s="4">
+      <c r="AI33" s="4">
         <v>0</v>
       </c>
-      <c r="AI33" s="16"/>
-      <c r="AJ33" s="17">
+      <c r="AJ33" s="16"/>
+      <c r="AK33" s="17">
         <v>0.87360000000000004</v>
       </c>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>0</v>
       </c>
@@ -4240,7 +4317,9 @@
       <c r="C34" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="D34" s="16"/>
+      <c r="D34" s="16">
+        <v>2</v>
+      </c>
       <c r="E34" s="16" t="s">
         <v>64</v>
       </c>
@@ -4296,7 +4375,7 @@
         <v>0.59279632568359375</v>
       </c>
       <c r="W34" s="17">
-        <v>12.46960957845052</v>
+        <v>124.696095784505</v>
       </c>
       <c r="X34" s="17">
         <v>-60.967918395996094</v>
@@ -4308,33 +4387,36 @@
         <v>10.0092573819168</v>
       </c>
       <c r="AA34" s="4">
+        <v>8.0269212271203857E-2</v>
+      </c>
+      <c r="AB34" s="4">
         <v>0</v>
       </c>
-      <c r="AB34" s="16"/>
-      <c r="AC34" s="17">
+      <c r="AC34" s="16"/>
+      <c r="AD34" s="17">
         <v>90.420717239379883</v>
       </c>
-      <c r="AD34" s="17">
+      <c r="AE34" s="17">
         <v>0.99890532531570386</v>
       </c>
-      <c r="AE34" s="17">
+      <c r="AF34" s="17">
         <v>179.33759307861328</v>
       </c>
-      <c r="AF34" s="17">
+      <c r="AG34" s="17">
         <v>80.870397567749023</v>
       </c>
-      <c r="AG34" s="17">
+      <c r="AH34" s="17">
         <v>3.61920166015625</v>
       </c>
-      <c r="AH34" s="4">
+      <c r="AI34" s="4">
         <v>0</v>
       </c>
-      <c r="AI34" s="16"/>
-      <c r="AJ34" s="17">
+      <c r="AJ34" s="16"/>
+      <c r="AK34" s="17">
         <v>0.12479999999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>0</v>
       </c>
@@ -4344,7 +4426,9 @@
       <c r="C35" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="D35" s="16"/>
+      <c r="D35" s="16">
+        <v>2</v>
+      </c>
       <c r="E35" s="16" t="s">
         <v>48</v>
       </c>
@@ -4412,31 +4496,34 @@
         <v>28.358970315624227</v>
       </c>
       <c r="AA35" s="4">
+        <v>0.84265277758912727</v>
+      </c>
+      <c r="AB35" s="4">
         <v>0</v>
       </c>
-      <c r="AB35" s="16"/>
-      <c r="AC35" s="16">
+      <c r="AC35" s="16"/>
+      <c r="AD35" s="16">
         <v>115.85807647705079</v>
       </c>
-      <c r="AD35" s="16">
+      <c r="AE35" s="16">
         <v>1.3819744675938068</v>
       </c>
-      <c r="AE35" s="16">
+      <c r="AF35" s="16">
         <v>225.51359558105469</v>
       </c>
-      <c r="AF35" s="16">
+      <c r="AG35" s="16">
         <v>59.654396057128906</v>
       </c>
-      <c r="AG35" s="16"/>
-      <c r="AH35" s="4">
+      <c r="AH35" s="16"/>
+      <c r="AI35" s="4">
         <v>0</v>
       </c>
-      <c r="AI35" s="16"/>
-      <c r="AJ35" s="16">
+      <c r="AJ35" s="16"/>
+      <c r="AK35" s="16">
         <v>1.248</v>
       </c>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>0</v>
       </c>
@@ -4446,7 +4533,9 @@
       <c r="C36" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="D36" s="16"/>
+      <c r="D36" s="16">
+        <v>2</v>
+      </c>
       <c r="E36" s="16" t="s">
         <v>65</v>
       </c>
@@ -4514,33 +4603,36 @@
         <v>34.398840828848918</v>
       </c>
       <c r="AA36" s="4">
+        <v>1.1147892193177849</v>
+      </c>
+      <c r="AB36" s="4">
         <v>0</v>
       </c>
-      <c r="AB36" s="16"/>
-      <c r="AC36" s="17">
+      <c r="AC36" s="16"/>
+      <c r="AD36" s="17">
         <v>113.76455535888672</v>
       </c>
-      <c r="AD36" s="17">
+      <c r="AE36" s="17">
         <v>0.95222826860390342</v>
       </c>
-      <c r="AE36" s="17">
+      <c r="AF36" s="17">
         <v>297.14878845214844</v>
       </c>
-      <c r="AF36" s="17">
+      <c r="AG36" s="17">
         <v>86.985597133636475</v>
       </c>
-      <c r="AG36" s="17">
+      <c r="AH36" s="17">
         <v>0.75872689938398363</v>
       </c>
-      <c r="AH36" s="4">
+      <c r="AI36" s="4">
         <v>0</v>
       </c>
-      <c r="AI36" s="16"/>
-      <c r="AJ36" s="17">
+      <c r="AJ36" s="16"/>
+      <c r="AK36" s="17">
         <v>1.1544000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>0</v>
       </c>
@@ -4550,7 +4642,9 @@
       <c r="C37" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="D37" s="16"/>
+      <c r="D37" s="16">
+        <v>2</v>
+      </c>
       <c r="E37" s="16" t="s">
         <v>66</v>
       </c>
@@ -4612,37 +4706,40 @@
         <v>-70.181278228759766</v>
       </c>
       <c r="Y37" s="17">
-        <v>-165.60092913592374</v>
+        <v>165.60092913592399</v>
       </c>
       <c r="Z37" s="17">
-        <v>50.252262471822824</v>
+        <v>20.252262471822799</v>
       </c>
       <c r="AA37" s="4">
+        <v>1.0202595229263018</v>
+      </c>
+      <c r="AB37" s="4">
         <v>0</v>
       </c>
-      <c r="AB37" s="16"/>
-      <c r="AC37" s="17">
+      <c r="AC37" s="16"/>
+      <c r="AD37" s="17">
         <v>97.606077194213867</v>
       </c>
-      <c r="AD37" s="17">
+      <c r="AE37" s="17">
         <v>2.055660764276098</v>
       </c>
-      <c r="AE37" s="17">
+      <c r="AF37" s="17">
         <v>136.53119850158691</v>
       </c>
-      <c r="AF37" s="17">
+      <c r="AG37" s="17">
         <v>35.443197518587112</v>
       </c>
-      <c r="AG37" s="16"/>
-      <c r="AH37" s="4">
+      <c r="AH37" s="16"/>
+      <c r="AI37" s="4">
         <v>0</v>
       </c>
-      <c r="AI37" s="16"/>
-      <c r="AJ37" s="17">
+      <c r="AJ37" s="16"/>
+      <c r="AK37" s="17">
         <v>0.93600000000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>0</v>
       </c>
@@ -4652,7 +4749,9 @@
       <c r="C38" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="D38" s="16"/>
+      <c r="D38" s="16">
+        <v>2</v>
+      </c>
       <c r="E38" s="16" t="s">
         <v>67</v>
       </c>
@@ -4708,7 +4807,7 @@
         <v>2.5271987915039063</v>
       </c>
       <c r="W38" s="17">
-        <v>27.41440709431965</v>
+        <v>274.14407094319603</v>
       </c>
       <c r="X38" s="17">
         <v>-64.877278518676761</v>
@@ -4720,31 +4819,34 @@
         <v>34.786725186667695</v>
       </c>
       <c r="AA38" s="4">
+        <v>0.12689213035679942</v>
+      </c>
+      <c r="AB38" s="4">
         <v>0</v>
       </c>
-      <c r="AB38" s="16"/>
-      <c r="AC38" s="17">
+      <c r="AC38" s="16"/>
+      <c r="AD38" s="17">
         <v>96.295678329467762</v>
       </c>
-      <c r="AD38" s="17">
+      <c r="AE38" s="17">
         <v>1.368265627645826</v>
       </c>
-      <c r="AE38" s="17">
+      <c r="AF38" s="17">
         <v>174.47039794921875</v>
       </c>
-      <c r="AF38" s="17">
+      <c r="AG38" s="17">
         <v>64.771199226379395</v>
       </c>
-      <c r="AG38" s="16"/>
-      <c r="AH38" s="4">
+      <c r="AH38" s="16"/>
+      <c r="AI38" s="4">
         <v>0</v>
       </c>
-      <c r="AI38" s="16"/>
-      <c r="AJ38" s="17">
+      <c r="AJ38" s="16"/>
+      <c r="AK38" s="17">
         <v>1.8404</v>
       </c>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>0</v>
       </c>
@@ -4754,7 +4856,9 @@
       <c r="C39" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="D39" s="16"/>
+      <c r="D39" s="16">
+        <v>3</v>
+      </c>
       <c r="E39" s="16" t="s">
         <v>68</v>
       </c>
@@ -4810,45 +4914,48 @@
         <v>1.1543960571289063</v>
       </c>
       <c r="W39" s="17">
-        <v>22.245602925618467</v>
+        <v>222.45602925618499</v>
       </c>
       <c r="X39" s="17">
         <v>-78.25271835327149</v>
       </c>
       <c r="Y39" s="17">
-        <v>873.32677524132293</v>
+        <v>87.332677524132293</v>
       </c>
       <c r="Z39" s="17">
         <v>11.763446148098266</v>
       </c>
       <c r="AA39" s="4">
+        <v>5.2879871080280937E-2</v>
+      </c>
+      <c r="AB39" s="4">
         <v>0</v>
       </c>
-      <c r="AB39" s="16"/>
-      <c r="AC39" s="17">
+      <c r="AC39" s="16"/>
+      <c r="AD39" s="17">
         <v>110.91911926269532</v>
       </c>
-      <c r="AD39" s="17">
+      <c r="AE39" s="17">
         <v>1.503601709681945</v>
       </c>
-      <c r="AE39" s="17">
+      <c r="AF39" s="17">
         <v>167.98079681396484</v>
       </c>
-      <c r="AF39" s="17">
+      <c r="AG39" s="17">
         <v>62.524801731109619</v>
       </c>
-      <c r="AG39" s="17">
+      <c r="AH39" s="17">
         <v>4.7736015319824219</v>
       </c>
-      <c r="AH39" s="4">
+      <c r="AI39" s="4">
         <v>0</v>
       </c>
-      <c r="AI39" s="16"/>
-      <c r="AJ39" s="17">
+      <c r="AJ39" s="16"/>
+      <c r="AK39" s="17">
         <v>0.83599999999999997</v>
       </c>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>0</v>
       </c>
@@ -4858,7 +4965,9 @@
       <c r="C40" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="D40" s="16"/>
+      <c r="D40" s="16">
+        <v>3</v>
+      </c>
       <c r="E40" s="16" t="s">
         <v>47</v>
       </c>
@@ -4914,47 +5023,78 @@
         <v>0.6864013671875</v>
       </c>
       <c r="W40" s="17">
-        <v>28.183993021647112</v>
+        <v>281.83993021647098</v>
       </c>
       <c r="X40" s="17">
         <v>-71.666399383544928</v>
       </c>
       <c r="Y40" s="17">
-        <v>675.98464604688286</v>
+        <v>67.598464604688303</v>
       </c>
       <c r="Z40" s="17">
         <v>11.150314314311965</v>
       </c>
       <c r="AA40" s="4">
+        <v>3.956257832503654E-2</v>
+      </c>
+      <c r="AB40" s="4">
         <v>0</v>
       </c>
-      <c r="AB40" s="16"/>
-      <c r="AC40" s="17">
+      <c r="AC40" s="16"/>
+      <c r="AD40" s="17">
         <v>93.693598175048834</v>
       </c>
-      <c r="AD40" s="17">
+      <c r="AE40" s="17">
         <v>1.3876212074342362</v>
       </c>
-      <c r="AE40" s="17">
+      <c r="AF40" s="17">
         <v>137.40479469299316</v>
       </c>
-      <c r="AF40" s="17">
+      <c r="AG40" s="17">
         <v>60.403200149536133</v>
       </c>
-      <c r="AG40" s="17">
+      <c r="AH40" s="17">
         <v>1.466400146484375</v>
       </c>
-      <c r="AH40" s="4">
+      <c r="AI40" s="4">
         <v>0</v>
       </c>
-      <c r="AI40" s="16"/>
-      <c r="AJ40" s="17">
+      <c r="AJ40" s="16"/>
+      <c r="AK40" s="17">
         <v>1.0296000000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="4"/>
-      <c r="D52" s="4"/>
+    <row r="45" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AA45" s="5"/>
+    </row>
+    <row r="46" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AA46" s="5"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>